<commit_message>
Updated SCG for VMware HCX 4.11.3
</commit_message>
<xml_diff>
--- a/security-configuration-hardening-guide/hcx/4.11/vmware-hcx-security-configuration-guide-411-controls.xlsx
+++ b/security-configuration-hardening-guide/hcx/4.11/vmware-hcx-security-configuration-guide-411-controls.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vmware\Projects\Security Configuration Guide\Security Configuration Guide 9\WORKING COPY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vmware\Projects\Security Configuration Guide\Security Configuration Guide 9\WORKING COPY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6A66F1-12EE-409C-BAC3-D3336880B1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1002AF13-4DE0-4387-90E6-60E9AC68C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="60" windowWidth="45555" windowHeight="19665" xr2:uid="{378E67A8-D089-4FA6-9DFE-D37B9D846B86}"/>
+    <workbookView xWindow="2004" yWindow="660" windowWidth="57816" windowHeight="20688" xr2:uid="{378E67A8-D089-4FA6-9DFE-D37B9D846B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="144">
   <si>
     <t>See the included documentation for important guidance and instructions.</t>
   </si>
@@ -113,9 +113,6 @@
     <t>PowerCLI Command Remediation</t>
   </si>
   <si>
-    <t>Base</t>
-  </si>
-  <si>
     <t>None.</t>
   </si>
   <si>
@@ -153,19 +150,6 @@
   </si>
   <si>
     <t>VAMI, Syslog</t>
-  </si>
-  <si>
-    <t>Maximum Length,
-Minimum Length,
-Character Requirements</t>
-  </si>
-  <si>
-    <t>Maximum Length: 64
-Minimum Length: 15
-At least 1 special 
-At least 1 uppercase
-At least 1 lowercase
-At least 1 numeric</t>
   </si>
   <si>
     <t>Deactivated</t>
@@ -367,9 +351,6 @@
     <t>This setting specifies the number of consecutive failed login attempts allowed for an HCX appliance (Manager or Connector) user account before the account is locked. This applies to both the admin and root user accounts.</t>
   </si>
   <si>
-    <t>All HCX appliances (Manager, Connector, and Service Mesh appliances) should be configured to forward their logs to a central, remote syslog server (e.g., VCF Operations for Logs or another SIEM solution). This ensures logs are preserved and aggregated for analysis. This is configured in the VAMI of the HCX Manager/Connector.</t>
-  </si>
-  <si>
     <t>A login banner should be configured for all HCX appliances (Manager and Connector) for both UI and SSH access. This banner should display an appropriate legal notice and warning, stating that the system is for authorized use only.</t>
   </si>
   <si>
@@ -379,16 +360,10 @@
     <t>All HCX components (Manager, Connector) and their paired VMware Cloud Foundation components (vCenter, ESX, NSX) must be running versions that are on the official VMware Cloud Foundation Product Interoperability Matrix.</t>
   </si>
   <si>
-    <t>All HCX appliances (Manager and Connector) and all related VMware Cloud Foundation components must have their clocks synchronized to a reliable, central Network Time Protocol (NTP) server.</t>
-  </si>
-  <si>
     <t>HCX appliance updates (for Manager and Connector) are managed via the appliance VAMI (port 9443). Administrators should regularly check for and apply the latest security patches and updates from the official VMware Cloud Foundation repository.</t>
   </si>
   <si>
     <t>Enabling network extension encryption increases CPU usage on the HCX Network Extension appliances.</t>
-  </si>
-  <si>
-    <t>(Get-CisService -Name "com.vmware.appliance.logging.forwarding").get()</t>
   </si>
   <si>
     <t>hcx-4.service-resilience-ne</t>
@@ -452,17 +427,6 @@
     <t>deny</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum Length: 8
-At least 1 special 
-At least 1 uppercase
-At least 1 lowercase
-At least 1 numeric
-</t>
-  </si>
-  <si>
     <t>/etc/pam.d/system-password</t>
   </si>
   <si>
@@ -470,9 +434,6 @@
   </si>
   <si>
     <t>Password expires</t>
-  </si>
-  <si>
-    <t>The HCX Manager appliance (Cloud and Connector) OS enforces complexity rules for local user accounts (admin, root). These rules should be configured to require a minimum length and a mix of uppercase, lowercase, numbers, and special characters.</t>
   </si>
   <si>
     <r>
@@ -585,13 +546,42 @@
     <t>VMware HCX Security Configuration Guide</t>
   </si>
   <si>
-    <t>Version 411-20251124-01</t>
-  </si>
-  <si>
     <t>Advanced</t>
   </si>
   <si>
     <t>Changes to password settings on the appliances may impact connectivity of other solutions, and may negatively impact automated deployment of subordinate HCX components, and will need to be reconfigured after an update or upgrade.</t>
+  </si>
+  <si>
+    <t>Version 411-20251201-01</t>
+  </si>
+  <si>
+    <t>HCX Manager</t>
+  </si>
+  <si>
+    <t>fail_interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">difok = 8
+minlen = 15
+dcredit = -1
+ucredit = -1
+lcredit = -1
+ocredit = -1
+dictcheck = 1
+enforce_for_root
+</t>
+  </si>
+  <si>
+    <t>The HCX Manager appliance (Cloud and Connector) OS enforces complexity rules for local user accounts (admin, root). These rules should be configured to require a minimum length and a mix of uppercase, lowercase, numbers, and special characters. These settings can be found in /etc/security/pwquality.conf.</t>
+  </si>
+  <si>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>All HCX appliances (Manager, Connector, and Service Mesh appliances) should be configured to forward their logs to a central, remote syslog server (e.g., VCF Operations for Logs or another SIEM solution). This ensures logs are preserved and aggregated for analysis. This is configured in the VAMI of the HCX Manager/Connector. Since HCX automatically deploys other component VMs from the HCX Manager, this setting must be configured on the HCX Manager prior to deployment.</t>
+  </si>
+  <si>
+    <t>All HCX appliances (Manager and Connector) and all related VMware Cloud Foundation components must have their clocks synchronized to a reliable, central Network Time Protocol (NTP) server. Since HCX automatically deploys other component VMs from the HCX Manager, this setting must be configured on the HCX Manager prior to deployment.</t>
   </si>
 </sst>
 </file>
@@ -764,16 +754,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -800,26 +790,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1486,6 +1456,26 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1536,31 +1526,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3695A651-C5D3-475E-B0F1-62D95BE20D6E}" name="Table1" displayName="Table1" ref="A1:S16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="0" headerRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3695A651-C5D3-475E-B0F1-62D95BE20D6E}" name="Table1" displayName="Table1" ref="A1:S16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20">
   <autoFilter ref="A1:S16" xr:uid="{3695A651-C5D3-475E-B0F1-62D95BE20D6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S16">
     <sortCondition ref="A2:A16"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{79C2AF0A-5390-4E9C-B0D5-8710D43BFCA8}" name="SCG ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{3A2F9A8A-E9C4-43A8-8594-3E2B9A6D5730}" name="Secure Controls_x000a_Framework ID" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{04C83ECD-7936-4E48-94C3-11B7501981A9}" name="DISA STIG ID" dataDxfId="17"/>
-    <tableColumn id="19" xr3:uid="{0C22C20C-5D4F-427F-9F5F-9E803CF25C95}" name="PCI DSS 4.0.1 ID" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{A908CAC9-5614-48A4-97C3-70CA9AC8DAFE}" name="Component_x000a_Name" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{E16C3EB7-CA62-41B0-81A3-43D994DC67B8}" name="Component Version" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{895DEAD4-BA35-4DEB-8BDB-962B3C89AD91}" name="Feature/Function" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{71DF3195-B3BB-4383-997D-CEDC42E35F5E}" name="Description/Title" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{426E1751-524C-44E0-BDFE-1D437FA86969}" name="Discussion" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{FE8DA64B-D7B6-4390-92F8-5979922A1CF8}" name="Potential Functional Impact if Default Value is Changed" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{B910FBF8-6292-4A9B-B845-87CB8C60FA3E}" name="Implementation_x000a_Priority" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{9BFF0C05-282D-4957-8499-73407BD57496}" name="Configuration Parameter" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{7AAC1EEF-6538-49BC-B64E-854CF38BD12C}" name="Installation Default Value" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{CD721173-154F-4E21-BC3D-DB2AC5F8A19C}" name="Baseline Suggested Value" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{AA97B976-1568-486E-88B7-7A4EA28C60EB}" name="Is the Default?" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{02A4FA27-33A4-43FE-84CE-5CD5C84AAA7A}" name="Action Needed" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{10B1F9B6-A49A-438E-AC43-8517B9CD2D77}" name="Setting Location" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{936E61C0-BF2D-4333-81AE-CF1CFBD1551E}" name="PowerCLI Command Assessment" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{5409B494-3A6E-419E-93EC-5CDA59C980DB}" name="PowerCLI Command Remediation" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{79C2AF0A-5390-4E9C-B0D5-8710D43BFCA8}" name="SCG ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{3A2F9A8A-E9C4-43A8-8594-3E2B9A6D5730}" name="Secure Controls_x000a_Framework ID" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{04C83ECD-7936-4E48-94C3-11B7501981A9}" name="DISA STIG ID" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{0C22C20C-5D4F-427F-9F5F-9E803CF25C95}" name="PCI DSS 4.0.1 ID" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{A908CAC9-5614-48A4-97C3-70CA9AC8DAFE}" name="Component_x000a_Name" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E16C3EB7-CA62-41B0-81A3-43D994DC67B8}" name="Component Version" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{895DEAD4-BA35-4DEB-8BDB-962B3C89AD91}" name="Feature/Function" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{71DF3195-B3BB-4383-997D-CEDC42E35F5E}" name="Description/Title" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{426E1751-524C-44E0-BDFE-1D437FA86969}" name="Discussion" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{FE8DA64B-D7B6-4390-92F8-5979922A1CF8}" name="Potential Functional Impact if Default Value is Changed" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{B910FBF8-6292-4A9B-B845-87CB8C60FA3E}" name="Implementation_x000a_Priority" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{9BFF0C05-282D-4957-8499-73407BD57496}" name="Configuration Parameter" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{7AAC1EEF-6538-49BC-B64E-854CF38BD12C}" name="Installation Default Value" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{CD721173-154F-4E21-BC3D-DB2AC5F8A19C}" name="Baseline Suggested Value" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{AA97B976-1568-486E-88B7-7A4EA28C60EB}" name="Is the Default?" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{02A4FA27-33A4-43FE-84CE-5CD5C84AAA7A}" name="Action Needed" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{10B1F9B6-A49A-438E-AC43-8517B9CD2D77}" name="Setting Location" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{936E61C0-BF2D-4333-81AE-CF1CFBD1551E}" name="PowerCLI Command Assessment" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{5409B494-3A6E-419E-93EC-5CDA59C980DB}" name="PowerCLI Command Remediation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1885,56 +1875,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D633219-EF3A-40A9-A077-828D0951CCAB}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="161.140625" customWidth="1"/>
+    <col min="1" max="1" width="161.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:1" ht="294" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="294" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
     </row>
   </sheetData>
@@ -1947,33 +1939,33 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="71.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="5" customWidth="1"/>
-    <col min="3" max="4" width="26.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="26.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="93.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="104.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="70.7109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="82.140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="47.42578125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.140625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="144.7109375" style="6" customWidth="1"/>
-    <col min="19" max="19" width="143.140625" style="6" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="8" width="93.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="104.88671875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="70.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="82.109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="30.44140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="47.44140625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.109375" style="6" customWidth="1"/>
+    <col min="18" max="18" width="144.6640625" style="6" customWidth="1"/>
+    <col min="19" max="19" width="143.109375" style="6" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -1984,7 +1976,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>7</v>
@@ -2032,514 +2024,514 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="O9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>25</v>
+      <c r="Q9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="12" t="s">
+    <row r="10" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="B10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S8" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="I10" s="10" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="M10" s="10">
         <v>86400</v>
@@ -2548,57 +2540,57 @@
         <v>0</v>
       </c>
       <c r="O10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="Q10" s="10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="M11" s="11">
         <v>3</v>
@@ -2607,234 +2599,234 @@
         <v>3</v>
       </c>
       <c r="O11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="Q11" s="10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>131</v>
+        <v>138</v>
+      </c>
+      <c r="M12" s="11">
+        <v>900</v>
       </c>
       <c r="N12" s="10">
         <v>900</v>
       </c>
-      <c r="O12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="11" t="s">
+      <c r="O12" s="10" t="s">
         <v>28</v>
       </c>
+      <c r="P12" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="Q12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="R12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="S12" s="10" t="s">
-        <v>25</v>
+      <c r="J14" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="M14" s="11">
+        <v>10</v>
+      </c>
+      <c r="N14" s="11">
+        <v>10</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="R13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="S13" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="10" t="s">
+    <row r="15" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="J14" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="L14" s="10" t="s">
+      <c r="H15" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="M14" s="11">
-        <v>5</v>
-      </c>
-      <c r="N14" s="11">
-        <v>5</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>144</v>
-      </c>
       <c r="L15" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="M15" s="11">
         <v>99999</v>
@@ -2843,78 +2835,78 @@
         <v>99999</v>
       </c>
       <c r="O15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="Q15" s="10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="R15" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q16" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="R16" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>